<commit_message>
created the MASTER model
Master model is composed of the top 50 point scorers in the NBA, accuracy ~68%(fantastic) also made it super streamline to use through various defs.
Added def to calculate how much to bet
</commit_message>
<xml_diff>
--- a/teamstats_.xlsx
+++ b/teamstats_.xlsx
@@ -322,12 +322,12 @@
     <t>Orlando</t>
   </si>
   <si>
+    <t>Milwaukee</t>
+  </si>
+  <si>
     <t>Dallas</t>
   </si>
   <si>
-    <t>Milwaukee</t>
-  </si>
-  <si>
     <t>Los Angeles</t>
   </si>
   <si>
@@ -412,12 +412,12 @@
     <t>Magic</t>
   </si>
   <si>
+    <t>Bucks</t>
+  </si>
+  <si>
     <t>Mavericks</t>
   </si>
   <si>
-    <t>Bucks</t>
-  </si>
-  <si>
     <t>Lakers</t>
   </si>
   <si>
@@ -502,12 +502,12 @@
     <t>magic</t>
   </si>
   <si>
+    <t>bucks</t>
+  </si>
+  <si>
     <t>mavericks</t>
   </si>
   <si>
-    <t>bucks</t>
-  </si>
-  <si>
     <t>lakers</t>
   </si>
   <si>
@@ -598,12 +598,12 @@
     <t>18-10</t>
   </si>
   <si>
+    <t>16-14</t>
+  </si>
+  <si>
     <t>15-13</t>
   </si>
   <si>
-    <t>16-14</t>
-  </si>
-  <si>
     <t xml:space="preserve">16-9 </t>
   </si>
   <si>
@@ -763,12 +763,12 @@
     <t>22-16</t>
   </si>
   <si>
+    <t>19-16</t>
+  </si>
+  <si>
     <t>21-16</t>
   </si>
   <si>
-    <t>19-16</t>
-  </si>
-  <si>
     <t>20-16</t>
   </si>
   <si>
@@ -1180,12 +1180,12 @@
     <t xml:space="preserve">12-2 </t>
   </si>
   <si>
+    <t xml:space="preserve">15-7 </t>
+  </si>
+  <si>
     <t xml:space="preserve">19-4 </t>
   </si>
   <si>
-    <t xml:space="preserve">15-7 </t>
-  </si>
-  <si>
     <t xml:space="preserve">16-3 </t>
   </si>
   <si>
@@ -1228,12 +1228,12 @@
     <t xml:space="preserve">1-10 </t>
   </si>
   <si>
+    <t xml:space="preserve">4-9  </t>
+  </si>
+  <si>
     <t xml:space="preserve">2-12 </t>
   </si>
   <si>
-    <t xml:space="preserve">4-9  </t>
-  </si>
-  <si>
     <t xml:space="preserve">4-12 </t>
   </si>
   <si>
@@ -1291,12 +1291,12 @@
     <t xml:space="preserve">14-2 </t>
   </si>
   <si>
+    <t xml:space="preserve">16-6 </t>
+  </si>
+  <si>
     <t xml:space="preserve">20-0 </t>
   </si>
   <si>
-    <t xml:space="preserve">16-6 </t>
-  </si>
-  <si>
     <t xml:space="preserve">18-2 </t>
   </si>
   <si>
@@ -1381,12 +1381,12 @@
     <t>21-12</t>
   </si>
   <si>
+    <t>18-14</t>
+  </si>
+  <si>
     <t>20-13</t>
   </si>
   <si>
-    <t>18-14</t>
-  </si>
-  <si>
     <t>20-11</t>
   </si>
   <si>
@@ -1546,10 +1546,10 @@
     <t xml:space="preserve">16-1 </t>
   </si>
   <si>
+    <t xml:space="preserve">19-6 </t>
+  </si>
+  <si>
     <t xml:space="preserve">17-7 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">19-6 </t>
   </si>
   <si>
     <t xml:space="preserve">15-5 </t>
@@ -3543,7 +3543,7 @@
         <v>507</v>
       </c>
       <c r="BF5" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="BG5" t="s">
         <v>283</v>
@@ -3785,7 +3785,7 @@
         <v>453</v>
       </c>
       <c r="BC6" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="BD6" t="s">
         <v>348</v>
@@ -4287,7 +4287,7 @@
         <v>495</v>
       </c>
       <c r="BE8" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="BF8" t="s">
         <v>275</v>
@@ -4633,7 +4633,7 @@
         <v>93</v>
       </c>
       <c r="D10">
-        <v>1610612742</v>
+        <v>1610612749</v>
       </c>
       <c r="E10" t="s">
         <v>102</v>
@@ -4645,7 +4645,7 @@
         <v>162</v>
       </c>
       <c r="H10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I10" t="s">
         <v>194</v>
@@ -4654,70 +4654,70 @@
         <v>5</v>
       </c>
       <c r="L10" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="M10" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="N10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O10">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="P10">
         <v>16</v>
       </c>
       <c r="Q10">
-        <v>0.5679999999999999</v>
+        <v>0.543</v>
       </c>
       <c r="R10">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="S10" t="s">
         <v>249</v>
       </c>
       <c r="T10" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="U10" t="s">
-        <v>281</v>
+        <v>301</v>
       </c>
       <c r="V10" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="W10" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="X10" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="Y10" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="Z10" t="s">
-        <v>234</v>
+        <v>337</v>
       </c>
       <c r="AA10" t="s">
-        <v>202</v>
+        <v>274</v>
       </c>
       <c r="AB10">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="AC10" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="AD10">
-        <v>5</v>
+        <v>-6</v>
       </c>
       <c r="AE10" t="s">
-        <v>363</v>
+        <v>372</v>
       </c>
       <c r="AF10">
         <v>7</v>
       </c>
       <c r="AG10">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AH10">
         <v>1</v>
@@ -4726,22 +4726,22 @@
         <v>376</v>
       </c>
       <c r="AJ10">
-        <v>-4</v>
+        <v>2</v>
       </c>
       <c r="AK10" t="s">
-        <v>366</v>
+        <v>373</v>
       </c>
       <c r="AL10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AM10" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="AN10">
-        <v>9.5</v>
+        <v>12.5</v>
       </c>
       <c r="AO10">
-        <v>3.5</v>
+        <v>12.5</v>
       </c>
       <c r="AP10">
         <v>0</v>
@@ -4774,73 +4774,73 @@
         <v>425</v>
       </c>
       <c r="AZ10" t="s">
-        <v>311</v>
+        <v>438</v>
       </c>
       <c r="BA10" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="BB10" t="s">
         <v>455</v>
       </c>
       <c r="BC10" t="s">
-        <v>478</v>
+        <v>463</v>
       </c>
       <c r="BD10" t="s">
-        <v>199</v>
+        <v>496</v>
       </c>
       <c r="BE10" t="s">
         <v>510</v>
       </c>
       <c r="BF10" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="BG10" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="BH10">
-        <v>116.4</v>
+        <v>113</v>
       </c>
       <c r="BI10">
-        <v>111.9</v>
+        <v>110.8</v>
       </c>
       <c r="BJ10">
-        <v>4.6</v>
+        <v>2.1</v>
       </c>
       <c r="BK10" t="s">
-        <v>541</v>
+        <v>194</v>
       </c>
       <c r="BL10" t="s">
-        <v>562</v>
+        <v>542</v>
       </c>
       <c r="BM10" t="s">
-        <v>568</v>
+        <v>554</v>
       </c>
       <c r="BN10" t="s">
-        <v>559</v>
+        <v>595</v>
       </c>
       <c r="BO10" t="s">
-        <v>194</v>
+        <v>561</v>
       </c>
       <c r="BP10" t="s">
+        <v>581</v>
+      </c>
+      <c r="BQ10" t="s">
+        <v>580</v>
+      </c>
+      <c r="BR10" t="s">
+        <v>566</v>
+      </c>
+      <c r="BS10" t="s">
+        <v>569</v>
+      </c>
+      <c r="CB10" t="s">
+        <v>565</v>
+      </c>
+      <c r="CC10" t="s">
+        <v>619</v>
+      </c>
+      <c r="CD10" t="s">
         <v>540</v>
-      </c>
-      <c r="BQ10" t="s">
-        <v>546</v>
-      </c>
-      <c r="BR10" t="s">
-        <v>564</v>
-      </c>
-      <c r="BS10" t="s">
-        <v>596</v>
-      </c>
-      <c r="CB10" t="s">
-        <v>561</v>
-      </c>
-      <c r="CC10" t="s">
-        <v>628</v>
-      </c>
-      <c r="CD10" t="s">
-        <v>629</v>
       </c>
       <c r="CE10" t="s">
         <v>249</v>
@@ -4855,22 +4855,22 @@
         <v>325</v>
       </c>
       <c r="CI10">
-        <v>4308</v>
+        <v>3954</v>
       </c>
       <c r="CJ10">
-        <v>4139</v>
+        <v>3879</v>
       </c>
       <c r="CK10">
-        <v>169</v>
+        <v>75</v>
       </c>
       <c r="CL10">
-        <v>11.5</v>
+        <v>12.5</v>
       </c>
       <c r="CN10">
         <v>0</v>
       </c>
       <c r="CO10" t="s">
-        <v>580</v>
+        <v>600</v>
       </c>
     </row>
     <row r="11" spans="1:93">
@@ -4884,7 +4884,7 @@
         <v>93</v>
       </c>
       <c r="D11">
-        <v>1610612749</v>
+        <v>1610612742</v>
       </c>
       <c r="E11" t="s">
         <v>103</v>
@@ -4896,7 +4896,7 @@
         <v>163</v>
       </c>
       <c r="H11" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="I11" t="s">
         <v>195</v>
@@ -4905,70 +4905,70 @@
         <v>5</v>
       </c>
       <c r="L11" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="M11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="N11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O11">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="P11">
         <v>16</v>
       </c>
       <c r="Q11">
-        <v>0.543</v>
+        <v>0.5679999999999999</v>
       </c>
       <c r="R11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="S11" t="s">
         <v>250</v>
       </c>
       <c r="T11" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="U11" t="s">
-        <v>301</v>
+        <v>281</v>
       </c>
       <c r="V11" t="s">
+        <v>319</v>
+      </c>
+      <c r="W11" t="s">
+        <v>317</v>
+      </c>
+      <c r="X11" t="s">
         <v>318</v>
       </c>
-      <c r="W11" t="s">
-        <v>316</v>
-      </c>
-      <c r="X11" t="s">
-        <v>316</v>
-      </c>
       <c r="Y11" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="Z11" t="s">
-        <v>337</v>
+        <v>234</v>
       </c>
       <c r="AA11" t="s">
-        <v>274</v>
+        <v>202</v>
       </c>
       <c r="AB11">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="AC11" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="AD11">
-        <v>-6</v>
+        <v>5</v>
       </c>
       <c r="AE11" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="AF11">
         <v>7</v>
       </c>
       <c r="AG11">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AH11">
         <v>1</v>
@@ -4977,22 +4977,22 @@
         <v>376</v>
       </c>
       <c r="AJ11">
-        <v>2</v>
+        <v>-4</v>
       </c>
       <c r="AK11" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
       <c r="AL11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AM11" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="AN11">
-        <v>12.5</v>
+        <v>9.5</v>
       </c>
       <c r="AO11">
-        <v>12.5</v>
+        <v>3.5</v>
       </c>
       <c r="AP11">
         <v>0</v>
@@ -5025,73 +5025,73 @@
         <v>426</v>
       </c>
       <c r="AZ11" t="s">
-        <v>438</v>
+        <v>311</v>
       </c>
       <c r="BA11" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="BB11" t="s">
         <v>456</v>
       </c>
       <c r="BC11" t="s">
-        <v>463</v>
+        <v>478</v>
       </c>
       <c r="BD11" t="s">
-        <v>496</v>
+        <v>199</v>
       </c>
       <c r="BE11" t="s">
         <v>511</v>
       </c>
       <c r="BF11" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="BG11" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="BH11">
-        <v>113</v>
+        <v>116.4</v>
       </c>
       <c r="BI11">
-        <v>110.8</v>
+        <v>111.9</v>
       </c>
       <c r="BJ11">
-        <v>2.1</v>
+        <v>4.6</v>
       </c>
       <c r="BK11" t="s">
+        <v>541</v>
+      </c>
+      <c r="BL11" t="s">
+        <v>562</v>
+      </c>
+      <c r="BM11" t="s">
+        <v>568</v>
+      </c>
+      <c r="BN11" t="s">
+        <v>559</v>
+      </c>
+      <c r="BO11" t="s">
         <v>195</v>
       </c>
-      <c r="BL11" t="s">
-        <v>542</v>
-      </c>
-      <c r="BM11" t="s">
-        <v>554</v>
-      </c>
-      <c r="BN11" t="s">
-        <v>595</v>
-      </c>
-      <c r="BO11" t="s">
+      <c r="BP11" t="s">
+        <v>540</v>
+      </c>
+      <c r="BQ11" t="s">
+        <v>546</v>
+      </c>
+      <c r="BR11" t="s">
+        <v>564</v>
+      </c>
+      <c r="BS11" t="s">
+        <v>596</v>
+      </c>
+      <c r="CB11" t="s">
         <v>561</v>
       </c>
-      <c r="BP11" t="s">
-        <v>581</v>
-      </c>
-      <c r="BQ11" t="s">
-        <v>580</v>
-      </c>
-      <c r="BR11" t="s">
-        <v>566</v>
-      </c>
-      <c r="BS11" t="s">
-        <v>569</v>
-      </c>
-      <c r="CB11" t="s">
-        <v>565</v>
-      </c>
       <c r="CC11" t="s">
-        <v>619</v>
+        <v>628</v>
       </c>
       <c r="CD11" t="s">
-        <v>540</v>
+        <v>629</v>
       </c>
       <c r="CE11" t="s">
         <v>250</v>
@@ -5106,22 +5106,22 @@
         <v>325</v>
       </c>
       <c r="CI11">
-        <v>3954</v>
+        <v>4308</v>
       </c>
       <c r="CJ11">
-        <v>3879</v>
+        <v>4139</v>
       </c>
       <c r="CK11">
-        <v>75</v>
+        <v>169</v>
       </c>
       <c r="CL11">
-        <v>12.5</v>
+        <v>11.5</v>
       </c>
       <c r="CN11">
         <v>0</v>
       </c>
       <c r="CO11" t="s">
-        <v>600</v>
+        <v>580</v>
       </c>
     </row>
     <row r="12" spans="1:93">
@@ -6531,7 +6531,7 @@
         <v>391</v>
       </c>
       <c r="BF17" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="BG17" t="s">
         <v>351</v>
@@ -6770,7 +6770,7 @@
         <v>340</v>
       </c>
       <c r="BB18" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="BC18" t="s">
         <v>256</v>
@@ -7526,7 +7526,7 @@
         <v>302</v>
       </c>
       <c r="BE21" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="BF21" t="s">
         <v>277</v>
@@ -8013,7 +8013,7 @@
         <v>333</v>
       </c>
       <c r="BB23" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="BC23" t="s">
         <v>487</v>
@@ -8025,7 +8025,7 @@
         <v>391</v>
       </c>
       <c r="BF23" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="BG23" t="s">
         <v>495</v>
@@ -9011,7 +9011,7 @@
         <v>490</v>
       </c>
       <c r="BD27" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="BE27" t="s">
         <v>237</v>
@@ -9268,7 +9268,7 @@
         <v>526</v>
       </c>
       <c r="BG28" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="BH28">
         <v>110.7</v>

</xml_diff>